<commit_message>
all implemented tests working
</commit_message>
<xml_diff>
--- a/profiles/gsq/scripts/geochemxl/tests/data/GeochemXL-v3.0-DRILLHOLE_LOCATION_02_invalid.xlsx
+++ b/profiles/gsq/scripts/geochemxl/tests/data/GeochemXL-v3.0-DRILLHOLE_LOCATION_02_invalid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/gsq/gsq-geochem/profiles/gsq/scripts/geochemxl/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F901F299-C81E-6945-8D7F-50ACD9232835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D0790A-96D4-1943-9C1F-72AB9BD6752F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="31900" windowHeight="20500" tabRatio="842" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1880" yWindow="500" windowWidth="31900" windowHeight="20500" tabRatio="842" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE_NOTES" sheetId="1" r:id="rId1"/>
@@ -92,10 +92,10 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="TANG Joseph - Personal View" guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1928" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="842" activeSheetId="13"/>
+    <customWorkbookView name="HOY Derek - Personal View" guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="917" activeSheetId="6" showComments="commIndAndComment"/>
+    <customWorkbookView name="KELLY Vance - Personal View" guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-678" windowWidth="2418" windowHeight="1368" tabRatio="842" activeSheetId="1" showComments="commIndAndComment"/>
     <customWorkbookView name="DAVIES Rhys - Personal View" guid="{853B6239-A439-411F-9927-AA08BF431DBB}" mergeInterval="0" personalView="1" xWindow="2926" yWindow="109" windowWidth="2700" windowHeight="1354" tabRatio="842" activeSheetId="9"/>
-    <customWorkbookView name="KELLY Vance - Personal View" guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-678" windowWidth="2418" windowHeight="1368" tabRatio="842" activeSheetId="1" showComments="commIndAndComment"/>
-    <customWorkbookView name="HOY Derek - Personal View" guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="917" activeSheetId="6" showComments="commIndAndComment"/>
-    <customWorkbookView name="TANG Joseph - Personal View" guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1928" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="842" activeSheetId="13"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="1288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="1289">
   <si>
     <t>FIELD</t>
   </si>
@@ -2057,15 +2057,6 @@
   </si>
   <si>
     <t>CURRENT_CLASS</t>
-  </si>
-  <si>
-    <t>EXPLORATION</t>
-  </si>
-  <si>
-    <t>APPRAISAL</t>
-  </si>
-  <si>
-    <t>DEVELOPMENT</t>
   </si>
   <si>
     <t>Data for the project and resource authority common to all other templates. This must be completed prior to filling other templates. All locations throughout the templates must be referenced to the coordinate system specified in this template.</t>
@@ -3899,18 +3890,6 @@
   </si>
   <si>
     <t>SAMPLE_PXRF</t>
-  </si>
-  <si>
-    <t>BEDROCK</t>
-  </si>
-  <si>
-    <t>TRENCHING</t>
-  </si>
-  <si>
-    <t>GEOTECHNICAL</t>
-  </si>
-  <si>
-    <t>METALLURGICAL</t>
   </si>
   <si>
     <t>VERSION 3.0</t>
@@ -4012,6 +3991,30 @@
   </si>
   <si>
     <t>PRE_COLLAR_METHOD</t>
+  </si>
+  <si>
+    <t>EXPLORATION CLASS</t>
+  </si>
+  <si>
+    <t>APPRAISAL CLASS</t>
+  </si>
+  <si>
+    <t>DEVELOPMENT CLASS</t>
+  </si>
+  <si>
+    <t>WATER CLASS</t>
+  </si>
+  <si>
+    <t>BEDROCK CLASS</t>
+  </si>
+  <si>
+    <t>TRENCHING CLASS</t>
+  </si>
+  <si>
+    <t>GEOTECHNICAL CLASS</t>
+  </si>
+  <si>
+    <t>METALLURGICAL CLASS</t>
   </si>
 </sst>
 </file>
@@ -5713,14 +5716,14 @@
     <row r="3" spans="2:23" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="13"/>
       <c r="C3" s="97" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="G3" s="14"/>
     </row>
     <row r="4" spans="2:23" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13"/>
       <c r="C4" s="121" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="D4" s="121"/>
       <c r="E4" s="121"/>
@@ -5740,14 +5743,14 @@
     <row r="7" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B7" s="13"/>
       <c r="C7" s="15" t="s">
-        <v>1265</v>
+        <v>1258</v>
       </c>
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B8" s="13"/>
       <c r="C8" s="15" t="s">
-        <v>1278</v>
+        <v>1271</v>
       </c>
       <c r="G8" s="14"/>
     </row>
@@ -5769,7 +5772,7 @@
     <row r="12" spans="2:23" ht="224.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="13"/>
       <c r="C12" s="128" t="s">
-        <v>1277</v>
+        <v>1270</v>
       </c>
       <c r="D12" s="129"/>
       <c r="E12" s="129"/>
@@ -5849,7 +5852,7 @@
         <v>55</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="F20" s="105" t="s">
         <v>3</v>
@@ -5952,10 +5955,10 @@
       <c r="B27" s="13"/>
       <c r="C27" s="133"/>
       <c r="D27" s="21" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="F27" s="105" t="s">
         <v>30</v>
@@ -6015,7 +6018,7 @@
         <v>608</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
       <c r="F31" s="105" t="s">
         <v>3</v>
@@ -6029,7 +6032,7 @@
         <v>607</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="F32" s="105" t="s">
         <v>3</v>
@@ -6040,10 +6043,10 @@
       <c r="B33" s="13"/>
       <c r="C33" s="133"/>
       <c r="D33" s="21" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>1257</v>
+        <v>1254</v>
       </c>
       <c r="F33" s="105" t="s">
         <v>3</v>
@@ -6054,10 +6057,10 @@
       <c r="B34" s="13"/>
       <c r="C34" s="133"/>
       <c r="D34" s="21" t="s">
-        <v>1254</v>
+        <v>1251</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="F34" s="105" t="s">
         <v>30</v>
@@ -6068,10 +6071,10 @@
       <c r="B35" s="13"/>
       <c r="C35" s="133"/>
       <c r="D35" s="21" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="F35" s="105" t="s">
         <v>3</v>
@@ -6096,7 +6099,7 @@
       <c r="B37" s="13"/>
       <c r="C37" s="133"/>
       <c r="D37" s="21" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
       <c r="E37" s="22" t="s">
         <v>611</v>
@@ -6110,10 +6113,10 @@
       <c r="B38" s="13"/>
       <c r="C38" s="133"/>
       <c r="D38" s="21" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="F38" s="22" t="s">
         <v>30</v>
@@ -6191,7 +6194,7 @@
         <v>3</v>
       </c>
       <c r="D46" s="122" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="E46" s="122"/>
       <c r="F46" s="123"/>
@@ -6227,7 +6230,7 @@
         <v>11</v>
       </c>
       <c r="D49" s="122" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="E49" s="122"/>
       <c r="F49" s="123"/>
@@ -6268,23 +6271,23 @@
   </sheetData>
   <sheetProtection sheet="1" selectLockedCells="1"/>
   <customSheetViews>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="70" showGridLines="0" topLeftCell="A20">
-      <selection activeCell="E25" sqref="E25"/>
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="70" showGridLines="0" topLeftCell="A43">
+      <selection activeCell="M20" sqref="M20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="80" showGridLines="0" topLeftCell="A34">
+      <selection activeCell="L8" sqref="L8"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="70" showGridLines="0" topLeftCell="A25">
       <selection activeCell="L19" sqref="L19"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="80" showGridLines="0" topLeftCell="A34">
-      <selection activeCell="L8" sqref="L8"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="70" showGridLines="0" topLeftCell="A43">
-      <selection activeCell="M20" sqref="M20"/>
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="70" showGridLines="0" topLeftCell="A20">
+      <selection activeCell="E25" sqref="E25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -6737,25 +6740,25 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <customSheetViews>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6795,10 +6798,10 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <customSheetViews>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" state="veryHidden">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" state="veryHidden">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" state="veryHidden">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" state="veryHidden">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -6814,7 +6817,7 @@
   <dimension ref="A1:X566"/>
   <sheetViews>
     <sheetView topLeftCell="C2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6848,7 +6851,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="90" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="G1" s="91"/>
     </row>
@@ -6875,7 +6878,7 @@
         <v>157</v>
       </c>
       <c r="N3" s="36" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="T3" s="36" t="s">
         <v>615</v>
@@ -6901,7 +6904,7 @@
         <v>58</v>
       </c>
       <c r="F4" s="99" t="s">
-        <v>1185</v>
+        <v>1182</v>
       </c>
       <c r="G4" s="99" t="s">
         <v>647</v>
@@ -6910,28 +6913,28 @@
         <v>168</v>
       </c>
       <c r="I4" s="99" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="J4" s="99" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
       <c r="K4" s="99" t="s">
-        <v>1189</v>
+        <v>1186</v>
       </c>
       <c r="L4" s="99" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="M4" s="99" t="s">
         <v>549</v>
       </c>
       <c r="N4" s="99" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="O4" s="99" t="s">
         <v>603</v>
       </c>
       <c r="P4" s="99" t="s">
-        <v>1209</v>
+        <v>1206</v>
       </c>
       <c r="Q4" s="99" t="s">
         <v>615</v>
@@ -6943,7 +6946,7 @@
         <v>601</v>
       </c>
       <c r="T4" s="99" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="U4" s="99" t="s">
         <v>192</v>
@@ -6955,7 +6958,7 @@
         <v>205</v>
       </c>
       <c r="X4" s="99" t="s">
-        <v>1266</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -6975,10 +6978,10 @@
         <v>631</v>
       </c>
       <c r="F5" s="106" t="s">
-        <v>1174</v>
+        <v>1171</v>
       </c>
       <c r="G5" s="106" t="s">
-        <v>648</v>
+        <v>1281</v>
       </c>
       <c r="H5" s="106" t="s">
         <v>169</v>
@@ -6990,34 +6993,34 @@
         <v>18</v>
       </c>
       <c r="K5" s="108" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="L5" s="106" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="M5" s="108" t="s">
         <v>550</v>
       </c>
       <c r="N5" s="106" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="O5" s="106" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="P5" s="109" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="Q5" s="106" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="R5" s="106" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="S5" s="106" t="s">
         <v>413</v>
       </c>
       <c r="T5" s="106" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="U5" s="106" t="s">
         <v>445</v>
@@ -7029,7 +7032,7 @@
         <v>198</v>
       </c>
       <c r="X5" s="106" t="s">
-        <v>1267</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
@@ -7046,52 +7049,52 @@
         <v>597</v>
       </c>
       <c r="E6" s="106" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="F6" s="106" t="s">
-        <v>1175</v>
+        <v>1172</v>
       </c>
       <c r="G6" s="106" t="s">
-        <v>649</v>
+        <v>1282</v>
       </c>
       <c r="H6" s="106" t="s">
         <v>170</v>
       </c>
       <c r="I6" s="106" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="J6" s="107" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="K6" s="108" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="L6" s="106" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="M6" s="108" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="N6" s="106" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="O6" s="106" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="P6" s="109" t="s">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="Q6" s="106" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="R6" s="106" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="S6" s="106" t="s">
         <v>605</v>
       </c>
       <c r="T6" s="106" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="U6" s="106" t="s">
         <v>465</v>
@@ -7103,7 +7106,7 @@
         <v>199</v>
       </c>
       <c r="X6" s="106" t="s">
-        <v>1268</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
@@ -7111,7 +7114,7 @@
         <v>61</v>
       </c>
       <c r="B7" s="118" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="C7" s="106" t="s">
         <v>20</v>
@@ -7120,13 +7123,13 @@
         <v>598</v>
       </c>
       <c r="E7" s="106" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="F7" s="106" t="s">
-        <v>1176</v>
+        <v>1173</v>
       </c>
       <c r="G7" s="106" t="s">
-        <v>650</v>
+        <v>1283</v>
       </c>
       <c r="H7" s="106" t="s">
         <v>171</v>
@@ -7138,37 +7141,37 @@
         <v>132</v>
       </c>
       <c r="K7" s="108" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="L7" s="106" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="M7" s="108" t="s">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="N7" s="106" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="O7" s="106" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="P7" s="109" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="Q7" s="106" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="R7" s="106" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="S7" s="106" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="T7" s="106" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="U7" s="106" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="V7" s="106" t="s">
         <v>627</v>
@@ -7177,7 +7180,7 @@
         <v>200</v>
       </c>
       <c r="X7" s="106" t="s">
-        <v>1269</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
@@ -7185,7 +7188,7 @@
         <v>62</v>
       </c>
       <c r="B8" s="118" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="C8" s="106" t="s">
         <v>645</v>
@@ -7194,13 +7197,13 @@
         <v>632</v>
       </c>
       <c r="E8" s="106" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="F8" s="106" t="s">
-        <v>1177</v>
+        <v>1174</v>
       </c>
       <c r="G8" s="106" t="s">
-        <v>149</v>
+        <v>1284</v>
       </c>
       <c r="H8" s="106" t="s">
         <v>172</v>
@@ -7209,37 +7212,37 @@
         <v>148</v>
       </c>
       <c r="J8" s="107" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="K8" s="108" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="L8" s="106" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="M8" s="106" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="N8" s="106" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="O8" s="106" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="P8" s="109" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="Q8" s="106" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="R8" s="106" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="S8" s="106" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="T8" s="106" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="U8" s="106" t="s">
         <v>447</v>
@@ -7255,7 +7258,7 @@
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="106"/>
       <c r="B9" s="118" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="C9" s="106" t="s">
         <v>22</v>
@@ -7264,13 +7267,13 @@
         <v>633</v>
       </c>
       <c r="E9" s="106" t="s">
-        <v>1200</v>
+        <v>1197</v>
       </c>
       <c r="F9" s="106" t="s">
-        <v>1178</v>
+        <v>1175</v>
       </c>
       <c r="G9" s="106" t="s">
-        <v>1261</v>
+        <v>1285</v>
       </c>
       <c r="H9" s="106" t="s">
         <v>646</v>
@@ -7282,37 +7285,37 @@
         <v>134</v>
       </c>
       <c r="K9" s="108" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="L9" s="106" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="M9" s="108" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
       <c r="N9" s="106" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="O9" s="106" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="P9" s="109" t="s">
-        <v>1214</v>
+        <v>1211</v>
       </c>
       <c r="Q9" s="106" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="R9" s="106" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="S9" s="106" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="T9" s="106" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="U9" s="106" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="V9" s="106" t="s">
         <v>629</v>
@@ -7325,7 +7328,7 @@
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="106"/>
       <c r="B10" s="118" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="C10" s="106"/>
       <c r="D10" s="106" t="s">
@@ -7335,49 +7338,49 @@
         <v>630</v>
       </c>
       <c r="F10" s="106" t="s">
-        <v>1179</v>
+        <v>1176</v>
       </c>
       <c r="G10" s="106" t="s">
-        <v>1262</v>
+        <v>1286</v>
       </c>
       <c r="H10" s="106" t="s">
         <v>184</v>
       </c>
       <c r="I10" s="106" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="J10" s="107" t="s">
         <v>133</v>
       </c>
       <c r="K10" s="108" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="L10" s="106" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="M10" s="108" t="s">
-        <v>1153</v>
+        <v>1150</v>
       </c>
       <c r="N10" s="106" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="O10" s="106" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="P10" s="109" t="s">
-        <v>1215</v>
+        <v>1212</v>
       </c>
       <c r="Q10" s="106" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="R10" s="106" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="S10" s="106" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="T10" s="106" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="U10" s="106" t="s">
         <v>448</v>
@@ -7391,58 +7394,58 @@
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="106"/>
       <c r="B11" s="118" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="C11" s="106"/>
       <c r="D11" s="106" t="s">
         <v>635</v>
       </c>
       <c r="E11" s="106" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="F11" s="106" t="s">
-        <v>1180</v>
+        <v>1177</v>
       </c>
       <c r="G11" s="106" t="s">
-        <v>1263</v>
+        <v>1287</v>
       </c>
       <c r="H11" s="106" t="s">
         <v>183</v>
       </c>
       <c r="I11" s="106"/>
       <c r="J11" s="107" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="K11" s="108" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="L11" s="106" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="M11" s="108" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
       <c r="N11" s="106" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="O11" s="106"/>
       <c r="P11" s="109" t="s">
-        <v>1216</v>
+        <v>1213</v>
       </c>
       <c r="Q11" s="106" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="R11" s="106" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="S11" s="106" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="T11" s="106" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="U11" s="106" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="V11" s="106"/>
       <c r="W11" s="106" t="s">
@@ -7453,56 +7456,56 @@
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="106"/>
       <c r="B12" s="118" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="C12" s="106"/>
       <c r="D12" s="106" t="s">
         <v>636</v>
       </c>
       <c r="E12" s="106" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="F12" s="106" t="s">
-        <v>1181</v>
+        <v>1178</v>
       </c>
       <c r="G12" s="106" t="s">
-        <v>1264</v>
+        <v>1288</v>
       </c>
       <c r="H12" s="106"/>
       <c r="I12" s="106"/>
       <c r="J12" s="107" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="K12" s="108" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="L12" s="106" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="M12" s="108" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="N12" s="106" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="O12" s="106"/>
       <c r="P12" s="109" t="s">
-        <v>1217</v>
+        <v>1214</v>
       </c>
       <c r="Q12" s="106" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="R12" s="106" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="S12" s="106" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="T12" s="106" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="U12" s="106" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="V12" s="106"/>
       <c r="W12" s="106"/>
@@ -7516,44 +7519,44 @@
       <c r="C13" s="106"/>
       <c r="D13" s="106"/>
       <c r="E13" s="106" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="F13" s="106" t="s">
-        <v>1182</v>
+        <v>1179</v>
       </c>
       <c r="G13" s="106"/>
       <c r="H13" s="106"/>
       <c r="I13" s="106"/>
       <c r="J13" s="107" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="K13" s="108" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="L13" s="106" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="M13" s="108" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="N13" s="106" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="O13" s="106"/>
       <c r="P13" s="109" t="s">
-        <v>1218</v>
+        <v>1215</v>
       </c>
       <c r="Q13" s="106" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="R13" s="106" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="S13" s="106" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="T13" s="106" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="U13" s="106" t="s">
         <v>449</v>
@@ -7570,40 +7573,40 @@
       <c r="C14" s="106"/>
       <c r="D14" s="106"/>
       <c r="E14" s="106" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="F14" s="106" t="s">
-        <v>1183</v>
+        <v>1180</v>
       </c>
       <c r="G14" s="106"/>
       <c r="H14" s="106"/>
       <c r="I14" s="106"/>
       <c r="J14" s="107"/>
       <c r="K14" s="108" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="L14" s="106" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="M14" s="106"/>
       <c r="N14" s="106" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="O14" s="106"/>
       <c r="P14" s="109" t="s">
-        <v>1219</v>
+        <v>1216</v>
       </c>
       <c r="Q14" s="106" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="R14" s="106" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="S14" s="106" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="T14" s="106" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="U14" s="106" t="s">
         <v>450</v>
@@ -7615,45 +7618,45 @@
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="106"/>
       <c r="B15" s="118" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="C15" s="106"/>
       <c r="D15" s="106"/>
       <c r="E15" s="106" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="F15" s="106" t="s">
-        <v>1184</v>
+        <v>1181</v>
       </c>
       <c r="G15" s="106"/>
       <c r="H15" s="106"/>
       <c r="I15" s="106"/>
       <c r="J15" s="110"/>
       <c r="K15" s="108" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="L15" s="106" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="M15" s="106"/>
       <c r="N15" s="106" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="O15" s="106"/>
       <c r="P15" s="109" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
       <c r="Q15" s="106" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="R15" s="106" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="S15" s="106" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="T15" s="106" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="U15" s="106" t="s">
         <v>451</v>
@@ -7665,7 +7668,7 @@
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="106"/>
       <c r="B16" s="118" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C16" s="106"/>
       <c r="D16" s="106"/>
@@ -7673,7 +7676,7 @@
         <v>637</v>
       </c>
       <c r="F16" s="106" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="G16" s="106"/>
       <c r="H16" s="106"/>
@@ -7683,25 +7686,25 @@
         <v>146</v>
       </c>
       <c r="L16" s="106" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="M16" s="106"/>
       <c r="N16" s="106" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="O16" s="106"/>
       <c r="P16" s="109" t="s">
-        <v>1221</v>
+        <v>1218</v>
       </c>
       <c r="Q16" s="106" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="R16" s="106" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="S16" s="106"/>
       <c r="T16" s="106" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="U16" s="106" t="s">
         <v>453</v>
@@ -7713,41 +7716,41 @@
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="106"/>
       <c r="B17" s="118" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="C17" s="106"/>
       <c r="D17" s="106" t="s">
         <v>599</v>
       </c>
       <c r="E17" s="106" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="F17" s="106" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
       <c r="G17" s="106"/>
       <c r="H17" s="106"/>
       <c r="I17" s="106"/>
       <c r="J17" s="106"/>
       <c r="K17" s="108" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="L17" s="106" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="M17" s="106"/>
       <c r="N17" s="106" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="O17" s="106"/>
       <c r="P17" s="109" t="s">
-        <v>1222</v>
+        <v>1219</v>
       </c>
       <c r="Q17" s="106" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="R17" s="106" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="S17" s="106"/>
       <c r="T17" s="106"/>
@@ -7761,41 +7764,41 @@
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="106"/>
       <c r="B18" s="118" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C18" s="106"/>
       <c r="D18" s="106" t="s">
         <v>599</v>
       </c>
       <c r="E18" s="106" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="F18" s="106" t="s">
-        <v>1186</v>
+        <v>1183</v>
       </c>
       <c r="G18" s="106"/>
       <c r="H18" s="106"/>
       <c r="I18" s="106"/>
       <c r="J18" s="106"/>
       <c r="K18" s="108" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="L18" s="106" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="M18" s="106"/>
       <c r="N18" s="106" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="O18" s="106"/>
       <c r="P18" s="109" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="Q18" s="106" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="R18" s="106" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="S18" s="106"/>
       <c r="T18" s="106"/>
@@ -7809,41 +7812,41 @@
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="106"/>
       <c r="B19" s="118" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="C19" s="106"/>
       <c r="D19" s="106" t="s">
         <v>599</v>
       </c>
       <c r="E19" s="106" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="F19" s="106" t="s">
-        <v>1187</v>
+        <v>1184</v>
       </c>
       <c r="G19" s="106"/>
       <c r="H19" s="106"/>
       <c r="I19" s="106"/>
       <c r="J19" s="106"/>
       <c r="K19" s="108" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
       <c r="L19" s="106" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="M19" s="106"/>
       <c r="N19" s="106" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="O19" s="106"/>
       <c r="P19" s="109" t="s">
-        <v>1224</v>
+        <v>1221</v>
       </c>
       <c r="Q19" s="106" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="R19" s="106" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="S19" s="106"/>
       <c r="T19" s="106"/>
@@ -7857,42 +7860,42 @@
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="106"/>
       <c r="B20" s="118" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="C20" s="106"/>
       <c r="D20" s="106"/>
       <c r="E20" s="106" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="F20" s="106" t="s">
-        <v>1188</v>
+        <v>1185</v>
       </c>
       <c r="G20" s="106"/>
       <c r="H20" s="106"/>
       <c r="I20" s="106"/>
       <c r="J20" s="106"/>
       <c r="K20" s="108" t="s">
-        <v>1134</v>
+        <v>1131</v>
       </c>
       <c r="L20" s="106" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="M20" s="106"/>
       <c r="N20" s="106"/>
       <c r="O20" s="106"/>
       <c r="P20" s="109" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="Q20" s="106" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="R20" s="106" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="S20" s="106"/>
       <c r="T20" s="106"/>
       <c r="U20" s="106" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="V20" s="106"/>
       <c r="W20" s="106"/>
@@ -7904,32 +7907,32 @@
       <c r="C21" s="106"/>
       <c r="D21" s="106"/>
       <c r="E21" s="106" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="F21" s="106" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="G21" s="106"/>
       <c r="H21" s="106"/>
       <c r="I21" s="106"/>
       <c r="J21" s="106"/>
       <c r="K21" s="108" t="s">
-        <v>1135</v>
+        <v>1132</v>
       </c>
       <c r="L21" s="106" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="M21" s="106"/>
       <c r="N21" s="106"/>
       <c r="O21" s="106"/>
       <c r="P21" s="109" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="Q21" s="106" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="R21" s="106" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="S21" s="106"/>
       <c r="T21" s="106"/>
@@ -7946,32 +7949,32 @@
       <c r="C22" s="106"/>
       <c r="D22" s="106"/>
       <c r="E22" s="106" t="s">
-        <v>1281</v>
+        <v>1274</v>
       </c>
       <c r="F22" s="106" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="G22" s="106"/>
       <c r="H22" s="106"/>
       <c r="I22" s="106"/>
       <c r="J22" s="106"/>
       <c r="K22" s="108" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
       <c r="L22" s="106" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="M22" s="106"/>
       <c r="N22" s="106"/>
       <c r="O22" s="106"/>
       <c r="P22" s="109" t="s">
-        <v>1227</v>
+        <v>1224</v>
       </c>
       <c r="Q22" s="106" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="R22" s="106" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="S22" s="106"/>
       <c r="T22" s="106"/>
@@ -7989,29 +7992,29 @@
       <c r="D23" s="106"/>
       <c r="E23" s="106"/>
       <c r="F23" s="106" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="G23" s="106"/>
       <c r="H23" s="106"/>
       <c r="I23" s="106"/>
       <c r="J23" s="106"/>
       <c r="K23" s="108" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="L23" s="106" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="M23" s="106"/>
       <c r="N23" s="106"/>
       <c r="O23" s="106"/>
       <c r="P23" s="109" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="Q23" s="106" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="R23" s="106" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="S23" s="106"/>
       <c r="T23" s="106"/>
@@ -8029,34 +8032,34 @@
       <c r="D24" s="106"/>
       <c r="E24" s="106"/>
       <c r="F24" s="106" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="G24" s="106"/>
       <c r="H24" s="106"/>
       <c r="I24" s="106"/>
       <c r="J24" s="106"/>
       <c r="K24" s="108" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
       <c r="L24" s="106" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="M24" s="106"/>
       <c r="N24" s="106"/>
       <c r="O24" s="106"/>
       <c r="P24" s="109" t="s">
-        <v>1228</v>
+        <v>1225</v>
       </c>
       <c r="Q24" s="106" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="R24" s="106" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="S24" s="106"/>
       <c r="T24" s="106"/>
       <c r="U24" s="106" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="V24" s="106"/>
       <c r="W24" s="106"/>
@@ -8069,34 +8072,34 @@
       <c r="D25" s="106"/>
       <c r="E25" s="106"/>
       <c r="F25" s="106" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="G25" s="106"/>
       <c r="H25" s="106"/>
       <c r="I25" s="106"/>
       <c r="J25" s="106"/>
       <c r="K25" s="108" t="s">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="L25" s="106" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="M25" s="106"/>
       <c r="N25" s="106"/>
       <c r="O25" s="106"/>
       <c r="P25" s="109" t="s">
-        <v>1229</v>
+        <v>1226</v>
       </c>
       <c r="Q25" s="106" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="R25" s="106" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="S25" s="106"/>
       <c r="T25" s="106"/>
       <c r="U25" s="106" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="V25" s="106"/>
       <c r="W25" s="106"/>
@@ -8109,34 +8112,34 @@
       <c r="D26" s="106"/>
       <c r="E26" s="106"/>
       <c r="F26" s="106" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="G26" s="106"/>
       <c r="H26" s="106"/>
       <c r="I26" s="106"/>
       <c r="J26" s="106"/>
       <c r="K26" s="108" t="s">
-        <v>1140</v>
+        <v>1137</v>
       </c>
       <c r="L26" s="106" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="M26" s="106"/>
       <c r="N26" s="106"/>
       <c r="O26" s="106"/>
       <c r="P26" s="109" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
       <c r="Q26" s="106" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="R26" s="106" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="S26" s="106"/>
       <c r="T26" s="106"/>
       <c r="U26" s="106" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="V26" s="106"/>
       <c r="W26" s="106"/>
@@ -8149,29 +8152,29 @@
       <c r="D27" s="106"/>
       <c r="E27" s="106"/>
       <c r="F27" s="106" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
       <c r="G27" s="106"/>
       <c r="H27" s="106"/>
       <c r="I27" s="106"/>
       <c r="J27" s="106"/>
       <c r="K27" s="108" t="s">
-        <v>1141</v>
+        <v>1138</v>
       </c>
       <c r="L27" s="106" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="M27" s="106"/>
       <c r="N27" s="106"/>
       <c r="O27" s="106"/>
       <c r="P27" s="109" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
       <c r="Q27" s="106" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="R27" s="106" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="S27" s="106"/>
       <c r="T27" s="106"/>
@@ -8189,7 +8192,7 @@
       <c r="D28" s="106"/>
       <c r="E28" s="106"/>
       <c r="F28" s="106" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="G28" s="106"/>
       <c r="H28" s="106"/>
@@ -8199,24 +8202,24 @@
         <v>134</v>
       </c>
       <c r="L28" s="106" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="M28" s="106"/>
       <c r="N28" s="106"/>
       <c r="O28" s="106"/>
       <c r="P28" s="109" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="Q28" s="106" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="R28" s="106" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="S28" s="106"/>
       <c r="T28" s="106"/>
       <c r="U28" s="106" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="V28" s="106"/>
       <c r="W28" s="106"/>
@@ -8229,34 +8232,34 @@
       <c r="D29" s="106"/>
       <c r="E29" s="106"/>
       <c r="F29" s="106" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="G29" s="106"/>
       <c r="H29" s="106"/>
       <c r="I29" s="106"/>
       <c r="J29" s="106"/>
       <c r="K29" s="108" t="s">
-        <v>1142</v>
+        <v>1139</v>
       </c>
       <c r="L29" s="106" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="M29" s="106"/>
       <c r="N29" s="106"/>
       <c r="O29" s="106"/>
       <c r="P29" s="109" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="Q29" s="106" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="R29" s="106" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="S29" s="106"/>
       <c r="T29" s="106"/>
       <c r="U29" s="106" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="V29" s="106"/>
       <c r="W29" s="106"/>
@@ -8269,34 +8272,34 @@
       <c r="D30" s="106"/>
       <c r="E30" s="106"/>
       <c r="F30" s="106" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="G30" s="106"/>
       <c r="H30" s="106"/>
       <c r="I30" s="106"/>
       <c r="J30" s="106"/>
       <c r="K30" s="108" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="L30" s="106" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="M30" s="106"/>
       <c r="N30" s="106"/>
       <c r="O30" s="106"/>
       <c r="P30" s="109" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="Q30" s="106" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="R30" s="106" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="S30" s="106"/>
       <c r="T30" s="106"/>
       <c r="U30" s="106" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="V30" s="106"/>
       <c r="W30" s="106"/>
@@ -8309,29 +8312,29 @@
       <c r="D31" s="106"/>
       <c r="E31" s="106"/>
       <c r="F31" s="106" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="G31" s="106"/>
       <c r="H31" s="106"/>
       <c r="I31" s="106"/>
       <c r="J31" s="106"/>
       <c r="K31" s="108" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
       <c r="L31" s="106" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="M31" s="106"/>
       <c r="N31" s="106"/>
       <c r="O31" s="106"/>
       <c r="P31" s="109" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="Q31" s="106" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="R31" s="106" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="S31" s="106"/>
       <c r="T31" s="106"/>
@@ -8349,29 +8352,29 @@
       <c r="D32" s="106"/>
       <c r="E32" s="106"/>
       <c r="F32" s="106" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
       <c r="G32" s="106"/>
       <c r="H32" s="106"/>
       <c r="I32" s="106"/>
       <c r="J32" s="106"/>
       <c r="K32" s="108" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
       <c r="L32" s="106" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="M32" s="106"/>
       <c r="N32" s="106"/>
       <c r="O32" s="106"/>
       <c r="P32" s="109" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
       <c r="Q32" s="106" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="R32" s="106" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="S32" s="106"/>
       <c r="T32" s="106"/>
@@ -8389,29 +8392,29 @@
       <c r="D33" s="106"/>
       <c r="E33" s="106"/>
       <c r="F33" s="106" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="G33" s="106"/>
       <c r="H33" s="106"/>
       <c r="I33" s="106"/>
       <c r="J33" s="106"/>
       <c r="K33" s="108" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
       <c r="L33" s="106" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="M33" s="106"/>
       <c r="N33" s="106"/>
       <c r="O33" s="106"/>
       <c r="P33" s="109" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
       <c r="Q33" s="106" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="R33" s="106" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="S33" s="106"/>
       <c r="T33" s="106"/>
@@ -8429,29 +8432,29 @@
       <c r="D34" s="106"/>
       <c r="E34" s="106"/>
       <c r="F34" s="106" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="G34" s="106"/>
       <c r="H34" s="106"/>
       <c r="I34" s="106"/>
       <c r="J34" s="106"/>
       <c r="K34" s="108" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="L34" s="106" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="M34" s="106"/>
       <c r="N34" s="106"/>
       <c r="O34" s="106"/>
       <c r="P34" s="109" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="Q34" s="106" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="R34" s="106" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="S34" s="106"/>
       <c r="T34" s="106"/>
@@ -8469,29 +8472,29 @@
       <c r="D35" s="106"/>
       <c r="E35" s="106"/>
       <c r="F35" s="106" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="G35" s="106"/>
       <c r="H35" s="106"/>
       <c r="I35" s="106"/>
       <c r="J35" s="106"/>
       <c r="K35" s="108" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="L35" s="106" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="M35" s="106"/>
       <c r="N35" s="106"/>
       <c r="O35" s="106"/>
       <c r="P35" s="109" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
       <c r="Q35" s="106" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="R35" s="106" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="S35" s="106"/>
       <c r="T35" s="106"/>
@@ -8509,34 +8512,34 @@
       <c r="D36" s="106"/>
       <c r="E36" s="106"/>
       <c r="F36" s="106" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
       <c r="G36" s="106"/>
       <c r="H36" s="106"/>
       <c r="I36" s="106"/>
       <c r="J36" s="106"/>
       <c r="K36" s="108" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="L36" s="106" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="M36" s="106"/>
       <c r="N36" s="106"/>
       <c r="O36" s="106"/>
       <c r="P36" s="109" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="Q36" s="106" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="R36" s="106" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="S36" s="106"/>
       <c r="T36" s="106"/>
       <c r="U36" s="106" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="V36" s="106"/>
       <c r="W36" s="106"/>
@@ -8549,34 +8552,34 @@
       <c r="D37" s="106"/>
       <c r="E37" s="106"/>
       <c r="F37" s="106" t="s">
-        <v>1190</v>
+        <v>1187</v>
       </c>
       <c r="G37" s="106"/>
       <c r="H37" s="106"/>
       <c r="I37" s="106"/>
       <c r="J37" s="106"/>
       <c r="K37" s="108" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="L37" s="106" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="M37" s="106"/>
       <c r="N37" s="106"/>
       <c r="O37" s="106"/>
       <c r="P37" s="109" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="Q37" s="106" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="R37" s="106" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="S37" s="106"/>
       <c r="T37" s="106"/>
       <c r="U37" s="106" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="V37" s="106"/>
       <c r="W37" s="106"/>
@@ -8589,34 +8592,34 @@
       <c r="D38" s="106"/>
       <c r="E38" s="106"/>
       <c r="F38" s="106" t="s">
-        <v>1191</v>
+        <v>1188</v>
       </c>
       <c r="G38" s="106"/>
       <c r="H38" s="106"/>
       <c r="I38" s="106"/>
       <c r="J38" s="106"/>
       <c r="K38" s="108" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
       <c r="L38" s="106" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="M38" s="106"/>
       <c r="N38" s="106"/>
       <c r="O38" s="106"/>
       <c r="P38" s="109" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
       <c r="Q38" s="106" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="R38" s="106" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="S38" s="106"/>
       <c r="T38" s="106"/>
       <c r="U38" s="106" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="V38" s="106"/>
       <c r="W38" s="106"/>
@@ -8629,7 +8632,7 @@
       <c r="D39" s="106"/>
       <c r="E39" s="106"/>
       <c r="F39" s="106" t="s">
-        <v>1192</v>
+        <v>1189</v>
       </c>
       <c r="G39" s="106"/>
       <c r="H39" s="106"/>
@@ -8637,24 +8640,24 @@
       <c r="J39" s="106"/>
       <c r="K39" s="106"/>
       <c r="L39" s="106" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="M39" s="106"/>
       <c r="N39" s="106"/>
       <c r="O39" s="106"/>
       <c r="P39" s="109" t="s">
-        <v>1243</v>
+        <v>1240</v>
       </c>
       <c r="Q39" s="106" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="R39" s="106" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="S39" s="106"/>
       <c r="T39" s="106"/>
       <c r="U39" s="106" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="V39" s="106"/>
       <c r="W39" s="106"/>
@@ -8667,7 +8670,7 @@
       <c r="D40" s="106"/>
       <c r="E40" s="106"/>
       <c r="F40" s="106" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
       <c r="G40" s="106"/>
       <c r="H40" s="106"/>
@@ -8675,24 +8678,24 @@
       <c r="J40" s="106"/>
       <c r="K40" s="106"/>
       <c r="L40" s="106" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="M40" s="106"/>
       <c r="N40" s="106"/>
       <c r="O40" s="106"/>
       <c r="P40" s="109" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="Q40" s="106" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="R40" s="106" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="S40" s="106"/>
       <c r="T40" s="106"/>
       <c r="U40" s="106" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="V40" s="106"/>
       <c r="W40" s="106"/>
@@ -8705,7 +8708,7 @@
       <c r="D41" s="106"/>
       <c r="E41" s="106"/>
       <c r="F41" s="106" t="s">
-        <v>1194</v>
+        <v>1191</v>
       </c>
       <c r="G41" s="106"/>
       <c r="H41" s="106"/>
@@ -8713,19 +8716,19 @@
       <c r="J41" s="106"/>
       <c r="K41" s="106"/>
       <c r="L41" s="106" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="M41" s="106"/>
       <c r="N41" s="106"/>
       <c r="O41" s="106"/>
       <c r="P41" s="109" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="Q41" s="106" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="R41" s="106" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="S41" s="106"/>
       <c r="T41" s="106"/>
@@ -8743,7 +8746,7 @@
       <c r="D42" s="106"/>
       <c r="E42" s="106"/>
       <c r="F42" s="106" t="s">
-        <v>1195</v>
+        <v>1192</v>
       </c>
       <c r="G42" s="106"/>
       <c r="H42" s="106"/>
@@ -8751,24 +8754,24 @@
       <c r="J42" s="106"/>
       <c r="K42" s="106"/>
       <c r="L42" s="106" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="M42" s="106"/>
       <c r="N42" s="106"/>
       <c r="O42" s="106"/>
       <c r="P42" s="109" t="s">
-        <v>1246</v>
+        <v>1243</v>
       </c>
       <c r="Q42" s="106" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="R42" s="106" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="S42" s="106"/>
       <c r="T42" s="106"/>
       <c r="U42" s="106" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="V42" s="106"/>
       <c r="W42" s="106"/>
@@ -8781,7 +8784,7 @@
       <c r="D43" s="106"/>
       <c r="E43" s="106"/>
       <c r="F43" s="106" t="s">
-        <v>1196</v>
+        <v>1193</v>
       </c>
       <c r="G43" s="106"/>
       <c r="H43" s="106"/>
@@ -8789,19 +8792,19 @@
       <c r="J43" s="106"/>
       <c r="K43" s="106"/>
       <c r="L43" s="106" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="M43" s="106"/>
       <c r="N43" s="106"/>
       <c r="O43" s="106"/>
       <c r="P43" s="109" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="Q43" s="106" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="R43" s="106" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="S43" s="106"/>
       <c r="T43" s="106"/>
@@ -8819,7 +8822,7 @@
       <c r="D44" s="106"/>
       <c r="E44" s="106"/>
       <c r="F44" s="106" t="s">
-        <v>1197</v>
+        <v>1194</v>
       </c>
       <c r="G44" s="106"/>
       <c r="H44" s="106"/>
@@ -8827,19 +8830,19 @@
       <c r="J44" s="106"/>
       <c r="K44" s="106"/>
       <c r="L44" s="106" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="M44" s="106"/>
       <c r="N44" s="106"/>
       <c r="O44" s="106"/>
       <c r="P44" s="109" t="s">
-        <v>1248</v>
+        <v>1245</v>
       </c>
       <c r="Q44" s="106" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="R44" s="106" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="S44" s="106"/>
       <c r="T44" s="106"/>
@@ -8857,7 +8860,7 @@
       <c r="D45" s="106"/>
       <c r="E45" s="106"/>
       <c r="F45" s="106" t="s">
-        <v>1198</v>
+        <v>1195</v>
       </c>
       <c r="G45" s="106"/>
       <c r="H45" s="106"/>
@@ -8865,24 +8868,24 @@
       <c r="J45" s="106"/>
       <c r="K45" s="106"/>
       <c r="L45" s="106" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="M45" s="106"/>
       <c r="N45" s="106"/>
       <c r="O45" s="106"/>
       <c r="P45" s="109" t="s">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="Q45" s="106" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="R45" s="106" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="S45" s="106"/>
       <c r="T45" s="106"/>
       <c r="U45" s="106" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="V45" s="106"/>
       <c r="W45" s="106"/>
@@ -8901,24 +8904,24 @@
       <c r="J46" s="106"/>
       <c r="K46" s="106"/>
       <c r="L46" s="106" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="M46" s="106"/>
       <c r="N46" s="106"/>
       <c r="O46" s="106"/>
       <c r="P46" s="109" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="Q46" s="106" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="R46" s="106" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="S46" s="106"/>
       <c r="T46" s="106"/>
       <c r="U46" s="106" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="V46" s="106"/>
       <c r="W46" s="106"/>
@@ -8937,19 +8940,19 @@
       <c r="J47" s="106"/>
       <c r="K47" s="106"/>
       <c r="L47" s="106" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="M47" s="106"/>
       <c r="N47" s="106"/>
       <c r="O47" s="106"/>
       <c r="P47" s="109" t="s">
-        <v>1251</v>
+        <v>1248</v>
       </c>
       <c r="Q47" s="106" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="R47" s="106" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="S47" s="106"/>
       <c r="T47" s="106"/>
@@ -8973,22 +8976,22 @@
       <c r="J48" s="106"/>
       <c r="K48" s="106"/>
       <c r="L48" s="106" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="M48" s="106"/>
       <c r="N48" s="106"/>
       <c r="O48" s="106"/>
       <c r="P48" s="106"/>
       <c r="Q48" s="106" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="R48" s="106" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="S48" s="106"/>
       <c r="T48" s="106"/>
       <c r="U48" s="106" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="V48" s="106"/>
       <c r="W48" s="106"/>
@@ -9007,22 +9010,22 @@
       <c r="J49" s="106"/>
       <c r="K49" s="106"/>
       <c r="L49" s="106" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="M49" s="106"/>
       <c r="N49" s="106"/>
       <c r="O49" s="106"/>
       <c r="P49" s="106"/>
       <c r="Q49" s="106" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="R49" s="106" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="S49" s="106"/>
       <c r="T49" s="106"/>
       <c r="U49" s="106" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="V49" s="106"/>
       <c r="W49" s="106"/>
@@ -9041,17 +9044,17 @@
       <c r="J50" s="106"/>
       <c r="K50" s="106"/>
       <c r="L50" s="106" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="M50" s="106"/>
       <c r="N50" s="106"/>
       <c r="O50" s="106"/>
       <c r="P50" s="106"/>
       <c r="Q50" s="106" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="R50" s="106" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="S50" s="106"/>
       <c r="T50" s="106"/>
@@ -9075,22 +9078,22 @@
       <c r="J51" s="106"/>
       <c r="K51" s="106"/>
       <c r="L51" s="106" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="M51" s="106"/>
       <c r="N51" s="106"/>
       <c r="O51" s="106"/>
       <c r="P51" s="106"/>
       <c r="Q51" s="106" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="R51" s="106" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="S51" s="106"/>
       <c r="T51" s="106"/>
       <c r="U51" s="106" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="V51" s="106"/>
       <c r="W51" s="106"/>
@@ -9109,17 +9112,17 @@
       <c r="J52" s="106"/>
       <c r="K52" s="106"/>
       <c r="L52" s="106" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="M52" s="106"/>
       <c r="N52" s="106"/>
       <c r="O52" s="106"/>
       <c r="P52" s="106"/>
       <c r="Q52" s="106" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="R52" s="106" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="S52" s="106"/>
       <c r="T52" s="106"/>
@@ -9143,22 +9146,22 @@
       <c r="J53" s="106"/>
       <c r="K53" s="106"/>
       <c r="L53" s="106" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="M53" s="106"/>
       <c r="N53" s="106"/>
       <c r="O53" s="106"/>
       <c r="P53" s="106"/>
       <c r="Q53" s="106" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="R53" s="106" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="S53" s="106"/>
       <c r="T53" s="106"/>
       <c r="U53" s="106" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="V53" s="106"/>
       <c r="W53" s="106"/>
@@ -9177,22 +9180,22 @@
       <c r="J54" s="106"/>
       <c r="K54" s="106"/>
       <c r="L54" s="106" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="M54" s="106"/>
       <c r="N54" s="106"/>
       <c r="O54" s="106"/>
       <c r="P54" s="106"/>
       <c r="Q54" s="106" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="R54" s="106" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="S54" s="106"/>
       <c r="T54" s="106"/>
       <c r="U54" s="106" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="V54" s="106"/>
       <c r="W54" s="106"/>
@@ -9211,17 +9214,17 @@
       <c r="J55" s="106"/>
       <c r="K55" s="106"/>
       <c r="L55" s="106" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="M55" s="106"/>
       <c r="N55" s="106"/>
       <c r="O55" s="106"/>
       <c r="P55" s="106"/>
       <c r="Q55" s="106" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="R55" s="106" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="S55" s="106"/>
       <c r="T55" s="106"/>
@@ -9245,17 +9248,17 @@
       <c r="J56" s="106"/>
       <c r="K56" s="106"/>
       <c r="L56" s="106" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="M56" s="106"/>
       <c r="N56" s="106"/>
       <c r="O56" s="106"/>
       <c r="P56" s="106"/>
       <c r="Q56" s="106" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="R56" s="106" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="S56" s="106"/>
       <c r="T56" s="106"/>
@@ -9279,22 +9282,22 @@
       <c r="J57" s="106"/>
       <c r="K57" s="106"/>
       <c r="L57" s="106" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="M57" s="106"/>
       <c r="N57" s="106"/>
       <c r="O57" s="106"/>
       <c r="P57" s="106"/>
       <c r="Q57" s="106" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="R57" s="106" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="S57" s="106"/>
       <c r="T57" s="106"/>
       <c r="U57" s="106" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="V57" s="106"/>
       <c r="W57" s="106"/>
@@ -9313,17 +9316,17 @@
       <c r="J58" s="106"/>
       <c r="K58" s="106"/>
       <c r="L58" s="106" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="M58" s="106"/>
       <c r="N58" s="106"/>
       <c r="O58" s="106"/>
       <c r="P58" s="106"/>
       <c r="Q58" s="106" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="R58" s="106" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="S58" s="106"/>
       <c r="T58" s="106"/>
@@ -9347,17 +9350,17 @@
       <c r="J59" s="106"/>
       <c r="K59" s="106"/>
       <c r="L59" s="106" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="M59" s="106"/>
       <c r="N59" s="106"/>
       <c r="O59" s="106"/>
       <c r="P59" s="106"/>
       <c r="Q59" s="106" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="R59" s="106" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="S59" s="106"/>
       <c r="T59" s="106"/>
@@ -9381,17 +9384,17 @@
       <c r="J60" s="106"/>
       <c r="K60" s="106"/>
       <c r="L60" s="106" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="M60" s="106"/>
       <c r="N60" s="106"/>
       <c r="O60" s="106"/>
       <c r="P60" s="106"/>
       <c r="Q60" s="106" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="R60" s="106" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="S60" s="106"/>
       <c r="T60" s="106"/>
@@ -9415,17 +9418,17 @@
       <c r="J61" s="106"/>
       <c r="K61" s="106"/>
       <c r="L61" s="106" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="M61" s="106"/>
       <c r="N61" s="106"/>
       <c r="O61" s="106"/>
       <c r="P61" s="106"/>
       <c r="Q61" s="106" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="R61" s="106" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="S61" s="106"/>
       <c r="T61" s="106"/>
@@ -9449,17 +9452,17 @@
       <c r="J62" s="106"/>
       <c r="K62" s="106"/>
       <c r="L62" s="106" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="M62" s="106"/>
       <c r="N62" s="106"/>
       <c r="O62" s="106"/>
       <c r="P62" s="106"/>
       <c r="Q62" s="106" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="R62" s="106" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="S62" s="106"/>
       <c r="T62" s="106"/>
@@ -9483,22 +9486,22 @@
       <c r="J63" s="106"/>
       <c r="K63" s="106"/>
       <c r="L63" s="106" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="M63" s="106"/>
       <c r="N63" s="106"/>
       <c r="O63" s="106"/>
       <c r="P63" s="106"/>
       <c r="Q63" s="106" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="R63" s="106" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="S63" s="106"/>
       <c r="T63" s="106"/>
       <c r="U63" s="106" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="V63" s="106"/>
       <c r="W63" s="106"/>
@@ -9517,17 +9520,17 @@
       <c r="J64" s="106"/>
       <c r="K64" s="106"/>
       <c r="L64" s="106" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="M64" s="106"/>
       <c r="N64" s="106"/>
       <c r="O64" s="106"/>
       <c r="P64" s="106"/>
       <c r="Q64" s="106" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="R64" s="106" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="S64" s="106"/>
       <c r="T64" s="106"/>
@@ -9551,7 +9554,7 @@
       <c r="J65" s="106"/>
       <c r="K65" s="106"/>
       <c r="L65" s="106" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="M65" s="106"/>
       <c r="N65" s="106"/>
@@ -9559,7 +9562,7 @@
       <c r="P65" s="106"/>
       <c r="Q65" s="106"/>
       <c r="R65" s="106" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="S65" s="106"/>
       <c r="T65" s="106"/>
@@ -9583,7 +9586,7 @@
       <c r="J66" s="106"/>
       <c r="K66" s="106"/>
       <c r="L66" s="106" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="M66" s="106"/>
       <c r="N66" s="106"/>
@@ -9591,12 +9594,12 @@
       <c r="P66" s="106"/>
       <c r="Q66" s="106"/>
       <c r="R66" s="106" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="S66" s="106"/>
       <c r="T66" s="106"/>
       <c r="U66" s="106" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="V66" s="106"/>
       <c r="W66" s="106"/>
@@ -9615,7 +9618,7 @@
       <c r="J67" s="106"/>
       <c r="K67" s="106"/>
       <c r="L67" s="106" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="M67" s="106"/>
       <c r="N67" s="106"/>
@@ -9623,7 +9626,7 @@
       <c r="P67" s="106"/>
       <c r="Q67" s="106"/>
       <c r="R67" s="106" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="S67" s="106"/>
       <c r="T67" s="106"/>
@@ -9647,7 +9650,7 @@
       <c r="J68" s="106"/>
       <c r="K68" s="106"/>
       <c r="L68" s="106" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="M68" s="106"/>
       <c r="N68" s="106"/>
@@ -9655,12 +9658,12 @@
       <c r="P68" s="106"/>
       <c r="Q68" s="106"/>
       <c r="R68" s="106" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="S68" s="106"/>
       <c r="T68" s="106"/>
       <c r="U68" s="106" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="V68" s="106"/>
       <c r="W68" s="106"/>
@@ -9679,7 +9682,7 @@
       <c r="J69" s="106"/>
       <c r="K69" s="106"/>
       <c r="L69" s="106" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="M69" s="106"/>
       <c r="N69" s="106"/>
@@ -9687,7 +9690,7 @@
       <c r="P69" s="106"/>
       <c r="Q69" s="106"/>
       <c r="R69" s="106" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="S69" s="106"/>
       <c r="T69" s="106"/>
@@ -9711,7 +9714,7 @@
       <c r="J70" s="106"/>
       <c r="K70" s="106"/>
       <c r="L70" s="106" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="M70" s="106"/>
       <c r="N70" s="106"/>
@@ -9719,7 +9722,7 @@
       <c r="P70" s="106"/>
       <c r="Q70" s="106"/>
       <c r="R70" s="106" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="S70" s="106"/>
       <c r="T70" s="106"/>
@@ -9743,7 +9746,7 @@
       <c r="J71" s="106"/>
       <c r="K71" s="106"/>
       <c r="L71" s="106" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="M71" s="106"/>
       <c r="N71" s="106"/>
@@ -9751,7 +9754,7 @@
       <c r="P71" s="106"/>
       <c r="Q71" s="106"/>
       <c r="R71" s="106" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="S71" s="106"/>
       <c r="T71" s="106"/>
@@ -9775,7 +9778,7 @@
       <c r="J72" s="106"/>
       <c r="K72" s="106"/>
       <c r="L72" s="106" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="M72" s="106"/>
       <c r="N72" s="106"/>
@@ -9783,12 +9786,12 @@
       <c r="P72" s="106"/>
       <c r="Q72" s="106"/>
       <c r="R72" s="106" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="S72" s="106"/>
       <c r="T72" s="106"/>
       <c r="U72" s="106" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="V72" s="106"/>
       <c r="W72" s="106"/>
@@ -9807,7 +9810,7 @@
       <c r="J73" s="106"/>
       <c r="K73" s="106"/>
       <c r="L73" s="106" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="M73" s="106"/>
       <c r="N73" s="106"/>
@@ -9815,7 +9818,7 @@
       <c r="P73" s="106"/>
       <c r="Q73" s="106"/>
       <c r="R73" s="106" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="S73" s="106"/>
       <c r="T73" s="106"/>
@@ -9839,7 +9842,7 @@
       <c r="J74" s="106"/>
       <c r="K74" s="106"/>
       <c r="L74" s="106" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="M74" s="106"/>
       <c r="N74" s="106"/>
@@ -9847,12 +9850,12 @@
       <c r="P74" s="106"/>
       <c r="Q74" s="106"/>
       <c r="R74" s="106" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="S74" s="106"/>
       <c r="T74" s="106"/>
       <c r="U74" s="106" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="V74" s="106"/>
       <c r="W74" s="106"/>
@@ -9871,7 +9874,7 @@
       <c r="J75" s="106"/>
       <c r="K75" s="106"/>
       <c r="L75" s="106" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="M75" s="106"/>
       <c r="N75" s="106"/>
@@ -9901,7 +9904,7 @@
       <c r="J76" s="106"/>
       <c r="K76" s="106"/>
       <c r="L76" s="106" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="M76" s="106"/>
       <c r="N76" s="106"/>
@@ -9931,7 +9934,7 @@
       <c r="J77" s="106"/>
       <c r="K77" s="106"/>
       <c r="L77" s="106" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="M77" s="106"/>
       <c r="N77" s="106"/>
@@ -9942,7 +9945,7 @@
       <c r="S77" s="106"/>
       <c r="T77" s="106"/>
       <c r="U77" s="106" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="V77" s="106"/>
       <c r="W77" s="106"/>
@@ -9961,7 +9964,7 @@
       <c r="J78" s="106"/>
       <c r="K78" s="106"/>
       <c r="L78" s="106" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="M78" s="106"/>
       <c r="N78" s="106"/>
@@ -9991,7 +9994,7 @@
       <c r="J79" s="106"/>
       <c r="K79" s="106"/>
       <c r="L79" s="106" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="M79" s="106"/>
       <c r="N79" s="106"/>
@@ -10002,7 +10005,7 @@
       <c r="S79" s="106"/>
       <c r="T79" s="106"/>
       <c r="U79" s="106" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="V79" s="106"/>
       <c r="W79" s="106"/>
@@ -10021,7 +10024,7 @@
       <c r="J80" s="106"/>
       <c r="K80" s="106"/>
       <c r="L80" s="106" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="M80" s="106"/>
       <c r="N80" s="106"/>
@@ -10032,7 +10035,7 @@
       <c r="S80" s="106"/>
       <c r="T80" s="106"/>
       <c r="U80" s="106" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="V80" s="106"/>
       <c r="W80" s="106"/>
@@ -10051,7 +10054,7 @@
       <c r="J81" s="106"/>
       <c r="K81" s="106"/>
       <c r="L81" s="106" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="M81" s="106"/>
       <c r="N81" s="106"/>
@@ -10081,7 +10084,7 @@
       <c r="J82" s="106"/>
       <c r="K82" s="106"/>
       <c r="L82" s="106" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="M82" s="106"/>
       <c r="N82" s="106"/>
@@ -10092,7 +10095,7 @@
       <c r="S82" s="106"/>
       <c r="T82" s="106"/>
       <c r="U82" s="106" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="V82" s="106"/>
       <c r="W82" s="106"/>
@@ -10111,7 +10114,7 @@
       <c r="J83" s="106"/>
       <c r="K83" s="106"/>
       <c r="L83" s="106" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="M83" s="106"/>
       <c r="N83" s="106"/>
@@ -10122,7 +10125,7 @@
       <c r="S83" s="106"/>
       <c r="T83" s="106"/>
       <c r="U83" s="106" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="V83" s="106"/>
       <c r="W83" s="106"/>
@@ -10141,7 +10144,7 @@
       <c r="J84" s="106"/>
       <c r="K84" s="106"/>
       <c r="L84" s="106" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="M84" s="106"/>
       <c r="N84" s="106"/>
@@ -10152,7 +10155,7 @@
       <c r="S84" s="106"/>
       <c r="T84" s="106"/>
       <c r="U84" s="106" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="V84" s="106"/>
       <c r="W84" s="106"/>
@@ -10171,7 +10174,7 @@
       <c r="J85" s="106"/>
       <c r="K85" s="106"/>
       <c r="L85" s="106" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="M85" s="106"/>
       <c r="N85" s="106"/>
@@ -10201,7 +10204,7 @@
       <c r="J86" s="106"/>
       <c r="K86" s="106"/>
       <c r="L86" s="106" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="M86" s="106"/>
       <c r="N86" s="106"/>
@@ -10231,7 +10234,7 @@
       <c r="J87" s="106"/>
       <c r="K87" s="106"/>
       <c r="L87" s="106" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="M87" s="106"/>
       <c r="N87" s="106"/>
@@ -10242,7 +10245,7 @@
       <c r="S87" s="106"/>
       <c r="T87" s="106"/>
       <c r="U87" s="106" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="V87" s="106"/>
       <c r="W87" s="106"/>
@@ -10261,7 +10264,7 @@
       <c r="J88" s="106"/>
       <c r="K88" s="106"/>
       <c r="L88" s="106" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="M88" s="106"/>
       <c r="N88" s="106"/>
@@ -10291,7 +10294,7 @@
       <c r="J89" s="106"/>
       <c r="K89" s="106"/>
       <c r="L89" s="106" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="M89" s="106"/>
       <c r="N89" s="106"/>
@@ -10321,7 +10324,7 @@
       <c r="J90" s="106"/>
       <c r="K90" s="106"/>
       <c r="L90" s="106" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="M90" s="106"/>
       <c r="N90" s="106"/>
@@ -10332,7 +10335,7 @@
       <c r="S90" s="106"/>
       <c r="T90" s="106"/>
       <c r="U90" s="106" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="V90" s="106"/>
       <c r="W90" s="106"/>
@@ -10351,7 +10354,7 @@
       <c r="J91" s="106"/>
       <c r="K91" s="106"/>
       <c r="L91" s="106" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="M91" s="106"/>
       <c r="N91" s="106"/>
@@ -10381,7 +10384,7 @@
       <c r="J92" s="106"/>
       <c r="K92" s="106"/>
       <c r="L92" s="106" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="M92" s="106"/>
       <c r="N92" s="106"/>
@@ -10411,7 +10414,7 @@
       <c r="J93" s="106"/>
       <c r="K93" s="106"/>
       <c r="L93" s="106" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="M93" s="106"/>
       <c r="N93" s="106"/>
@@ -10441,7 +10444,7 @@
       <c r="J94" s="106"/>
       <c r="K94" s="106"/>
       <c r="L94" s="106" t="s">
-        <v>1084</v>
+        <v>1081</v>
       </c>
       <c r="M94" s="106"/>
       <c r="N94" s="106"/>
@@ -10452,7 +10455,7 @@
       <c r="S94" s="106"/>
       <c r="T94" s="106"/>
       <c r="U94" s="106" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="V94" s="106"/>
       <c r="W94" s="106"/>
@@ -10471,7 +10474,7 @@
       <c r="J95" s="106"/>
       <c r="K95" s="106"/>
       <c r="L95" s="106" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="M95" s="106"/>
       <c r="N95" s="106"/>
@@ -10482,7 +10485,7 @@
       <c r="S95" s="106"/>
       <c r="T95" s="106"/>
       <c r="U95" s="106" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="V95" s="106"/>
       <c r="W95" s="106"/>
@@ -10501,7 +10504,7 @@
       <c r="J96" s="106"/>
       <c r="K96" s="106"/>
       <c r="L96" s="106" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="M96" s="106"/>
       <c r="N96" s="106"/>
@@ -10531,7 +10534,7 @@
       <c r="J97" s="106"/>
       <c r="K97" s="106"/>
       <c r="L97" s="106" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="M97" s="106"/>
       <c r="N97" s="106"/>
@@ -10561,7 +10564,7 @@
       <c r="J98" s="106"/>
       <c r="K98" s="106"/>
       <c r="L98" s="106" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="M98" s="106"/>
       <c r="N98" s="106"/>
@@ -10572,7 +10575,7 @@
       <c r="S98" s="106"/>
       <c r="T98" s="106"/>
       <c r="U98" s="106" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="V98" s="106"/>
       <c r="W98" s="106"/>
@@ -10591,7 +10594,7 @@
       <c r="J99" s="106"/>
       <c r="K99" s="106"/>
       <c r="L99" s="106" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="M99" s="106"/>
       <c r="N99" s="106"/>
@@ -10602,7 +10605,7 @@
       <c r="S99" s="106"/>
       <c r="T99" s="106"/>
       <c r="U99" s="106" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="V99" s="106"/>
       <c r="W99" s="106"/>
@@ -10621,7 +10624,7 @@
       <c r="J100" s="106"/>
       <c r="K100" s="106"/>
       <c r="L100" s="106" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="M100" s="106"/>
       <c r="N100" s="106"/>
@@ -10632,7 +10635,7 @@
       <c r="S100" s="106"/>
       <c r="T100" s="106"/>
       <c r="U100" s="106" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="V100" s="106"/>
       <c r="W100" s="106"/>
@@ -10651,7 +10654,7 @@
       <c r="J101" s="106"/>
       <c r="K101" s="106"/>
       <c r="L101" s="106" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="M101" s="106"/>
       <c r="N101" s="106"/>
@@ -10681,7 +10684,7 @@
       <c r="J102" s="106"/>
       <c r="K102" s="106"/>
       <c r="L102" s="106" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="M102" s="106"/>
       <c r="N102" s="106"/>
@@ -10711,7 +10714,7 @@
       <c r="J103" s="106"/>
       <c r="K103" s="106"/>
       <c r="L103" s="106" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="M103" s="106"/>
       <c r="N103" s="106"/>
@@ -10741,7 +10744,7 @@
       <c r="J104" s="106"/>
       <c r="K104" s="106"/>
       <c r="L104" s="106" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
       <c r="M104" s="106"/>
       <c r="N104" s="106"/>
@@ -10752,7 +10755,7 @@
       <c r="S104" s="106"/>
       <c r="T104" s="106"/>
       <c r="U104" s="106" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="V104" s="106"/>
       <c r="W104" s="106"/>
@@ -10771,7 +10774,7 @@
       <c r="J105" s="106"/>
       <c r="K105" s="106"/>
       <c r="L105" s="106" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="M105" s="106"/>
       <c r="N105" s="106"/>
@@ -10782,7 +10785,7 @@
       <c r="S105" s="106"/>
       <c r="T105" s="106"/>
       <c r="U105" s="106" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="V105" s="106"/>
       <c r="W105" s="106"/>
@@ -10801,7 +10804,7 @@
       <c r="J106" s="106"/>
       <c r="K106" s="106"/>
       <c r="L106" s="106" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="M106" s="106"/>
       <c r="N106" s="106"/>
@@ -10812,7 +10815,7 @@
       <c r="S106" s="106"/>
       <c r="T106" s="106"/>
       <c r="U106" s="106" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="V106" s="106"/>
       <c r="W106" s="106"/>
@@ -10831,7 +10834,7 @@
       <c r="J107" s="106"/>
       <c r="K107" s="106"/>
       <c r="L107" s="106" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="M107" s="106"/>
       <c r="N107" s="106"/>
@@ -10870,7 +10873,7 @@
       <c r="S108" s="106"/>
       <c r="T108" s="106"/>
       <c r="U108" s="106" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="V108" s="106"/>
       <c r="W108" s="106"/>
@@ -11038,7 +11041,7 @@
       <c r="S114" s="106"/>
       <c r="T114" s="106"/>
       <c r="U114" s="106" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="V114" s="106"/>
       <c r="W114" s="106"/>
@@ -11066,7 +11069,7 @@
       <c r="S115" s="106"/>
       <c r="T115" s="106"/>
       <c r="U115" s="106" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="V115" s="106"/>
       <c r="W115" s="106"/>
@@ -11122,7 +11125,7 @@
       <c r="S117" s="106"/>
       <c r="T117" s="106"/>
       <c r="U117" s="106" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="V117" s="106"/>
       <c r="W117" s="106"/>
@@ -11178,7 +11181,7 @@
       <c r="S119" s="106"/>
       <c r="T119" s="106"/>
       <c r="U119" s="106" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="V119" s="106"/>
       <c r="W119" s="106"/>
@@ -11206,7 +11209,7 @@
       <c r="S120" s="106"/>
       <c r="T120" s="106"/>
       <c r="U120" s="106" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="V120" s="106"/>
       <c r="W120" s="106"/>
@@ -11234,7 +11237,7 @@
       <c r="S121" s="106"/>
       <c r="T121" s="106"/>
       <c r="U121" s="106" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="V121" s="106"/>
       <c r="W121" s="106"/>
@@ -11290,7 +11293,7 @@
       <c r="S123" s="106"/>
       <c r="T123" s="106"/>
       <c r="U123" s="106" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="V123" s="106"/>
       <c r="W123" s="106"/>
@@ -11318,7 +11321,7 @@
       <c r="S124" s="106"/>
       <c r="T124" s="106"/>
       <c r="U124" s="106" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="V124" s="106"/>
       <c r="W124" s="106"/>
@@ -11374,7 +11377,7 @@
       <c r="S126" s="106"/>
       <c r="T126" s="106"/>
       <c r="U126" s="106" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="V126" s="106"/>
       <c r="W126" s="106"/>
@@ -11458,7 +11461,7 @@
       <c r="S129" s="106"/>
       <c r="T129" s="106"/>
       <c r="U129" s="106" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="V129" s="106"/>
       <c r="W129" s="106"/>
@@ -11486,7 +11489,7 @@
       <c r="S130" s="106"/>
       <c r="T130" s="106"/>
       <c r="U130" s="106" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="V130" s="106"/>
       <c r="W130" s="106"/>
@@ -11514,7 +11517,7 @@
       <c r="S131" s="106"/>
       <c r="T131" s="106"/>
       <c r="U131" s="106" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="V131" s="106"/>
       <c r="W131" s="106"/>
@@ -11542,7 +11545,7 @@
       <c r="S132" s="106"/>
       <c r="T132" s="106"/>
       <c r="U132" s="106" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="V132" s="106"/>
       <c r="W132" s="106"/>
@@ -11626,7 +11629,7 @@
       <c r="S135" s="106"/>
       <c r="T135" s="106"/>
       <c r="U135" s="106" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="V135" s="106"/>
       <c r="W135" s="106"/>
@@ -11654,7 +11657,7 @@
       <c r="S136" s="106"/>
       <c r="T136" s="106"/>
       <c r="U136" s="106" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="V136" s="106"/>
       <c r="W136" s="106"/>
@@ -11738,7 +11741,7 @@
       <c r="S139" s="106"/>
       <c r="T139" s="106"/>
       <c r="U139" s="106" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="V139" s="106"/>
       <c r="W139" s="106"/>
@@ -11766,7 +11769,7 @@
       <c r="S140" s="106"/>
       <c r="T140" s="106"/>
       <c r="U140" s="106" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="V140" s="106"/>
       <c r="W140" s="106"/>
@@ -11822,7 +11825,7 @@
       <c r="S142" s="106"/>
       <c r="T142" s="106"/>
       <c r="U142" s="106" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="V142" s="106"/>
       <c r="W142" s="106"/>
@@ -11878,7 +11881,7 @@
       <c r="S144" s="106"/>
       <c r="T144" s="106"/>
       <c r="U144" s="106" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="V144" s="106"/>
       <c r="W144" s="106"/>
@@ -11990,7 +11993,7 @@
       <c r="S148" s="106"/>
       <c r="T148" s="106"/>
       <c r="U148" s="106" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="V148" s="106"/>
       <c r="W148" s="106"/>
@@ -12018,7 +12021,7 @@
       <c r="S149" s="106"/>
       <c r="T149" s="106"/>
       <c r="U149" s="106" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="V149" s="106"/>
       <c r="W149" s="106"/>
@@ -12102,7 +12105,7 @@
       <c r="S152" s="106"/>
       <c r="T152" s="106"/>
       <c r="U152" s="106" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="V152" s="106"/>
       <c r="W152" s="106"/>
@@ -12158,7 +12161,7 @@
       <c r="S154" s="106"/>
       <c r="T154" s="106"/>
       <c r="U154" s="106" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="V154" s="106"/>
       <c r="W154" s="106"/>
@@ -12214,7 +12217,7 @@
       <c r="S156" s="106"/>
       <c r="T156" s="106"/>
       <c r="U156" s="106" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="V156" s="106"/>
       <c r="W156" s="106"/>
@@ -12326,7 +12329,7 @@
       <c r="S160" s="106"/>
       <c r="T160" s="106"/>
       <c r="U160" s="106" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="V160" s="106"/>
       <c r="W160" s="106"/>
@@ -12466,7 +12469,7 @@
       <c r="S165" s="106"/>
       <c r="T165" s="106"/>
       <c r="U165" s="106" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="V165" s="106"/>
       <c r="W165" s="106"/>
@@ -12858,7 +12861,7 @@
       <c r="S179" s="106"/>
       <c r="T179" s="106"/>
       <c r="U179" s="106" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="V179" s="106"/>
       <c r="W179" s="106"/>
@@ -12886,7 +12889,7 @@
       <c r="S180" s="106"/>
       <c r="T180" s="106"/>
       <c r="U180" s="106" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="V180" s="106"/>
       <c r="W180" s="106"/>
@@ -12914,7 +12917,7 @@
       <c r="S181" s="106"/>
       <c r="T181" s="106"/>
       <c r="U181" s="106" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="V181" s="106"/>
       <c r="W181" s="106"/>
@@ -13166,7 +13169,7 @@
       <c r="S190" s="106"/>
       <c r="T190" s="106"/>
       <c r="U190" s="106" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="V190" s="106"/>
       <c r="W190" s="106"/>
@@ -13362,7 +13365,7 @@
       <c r="S197" s="106"/>
       <c r="T197" s="106"/>
       <c r="U197" s="106" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="V197" s="106"/>
       <c r="W197" s="106"/>
@@ -13390,7 +13393,7 @@
       <c r="S198" s="106"/>
       <c r="T198" s="106"/>
       <c r="U198" s="106" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="V198" s="106"/>
       <c r="W198" s="106"/>
@@ -13418,7 +13421,7 @@
       <c r="S199" s="106"/>
       <c r="T199" s="106"/>
       <c r="U199" s="106" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="V199" s="106"/>
       <c r="W199" s="106"/>
@@ -13558,7 +13561,7 @@
       <c r="S204" s="106"/>
       <c r="T204" s="106"/>
       <c r="U204" s="106" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="V204" s="106"/>
       <c r="W204" s="106"/>
@@ -13726,7 +13729,7 @@
       <c r="S210" s="106"/>
       <c r="T210" s="106"/>
       <c r="U210" s="106" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="V210" s="106"/>
       <c r="W210" s="106"/>
@@ -13782,7 +13785,7 @@
       <c r="S212" s="106"/>
       <c r="T212" s="106"/>
       <c r="U212" s="106" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="V212" s="106"/>
       <c r="W212" s="106"/>
@@ -13838,7 +13841,7 @@
       <c r="S214" s="106"/>
       <c r="T214" s="106"/>
       <c r="U214" s="106" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="V214" s="106"/>
       <c r="W214" s="106"/>
@@ -13866,7 +13869,7 @@
       <c r="S215" s="106"/>
       <c r="T215" s="106"/>
       <c r="U215" s="106" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="V215" s="106"/>
       <c r="W215" s="106"/>
@@ -13894,7 +13897,7 @@
       <c r="S216" s="106"/>
       <c r="T216" s="106"/>
       <c r="U216" s="106" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="V216" s="106"/>
       <c r="W216" s="106"/>
@@ -14090,7 +14093,7 @@
       <c r="S223" s="106"/>
       <c r="T223" s="106"/>
       <c r="U223" s="106" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="V223" s="106"/>
       <c r="W223" s="106"/>
@@ -14146,7 +14149,7 @@
       <c r="S225" s="106"/>
       <c r="T225" s="106"/>
       <c r="U225" s="106" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="V225" s="106"/>
       <c r="W225" s="106"/>
@@ -14230,7 +14233,7 @@
       <c r="S228" s="106"/>
       <c r="T228" s="106"/>
       <c r="U228" s="106" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="V228" s="106"/>
       <c r="W228" s="106"/>
@@ -14762,7 +14765,7 @@
       <c r="S247" s="106"/>
       <c r="T247" s="106"/>
       <c r="U247" s="106" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="V247" s="106"/>
       <c r="W247" s="106"/>
@@ -14902,7 +14905,7 @@
       <c r="S252" s="106"/>
       <c r="T252" s="106"/>
       <c r="U252" s="106" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="V252" s="106"/>
       <c r="W252" s="106"/>
@@ -14930,7 +14933,7 @@
       <c r="S253" s="106"/>
       <c r="T253" s="106"/>
       <c r="U253" s="106" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="V253" s="106"/>
       <c r="W253" s="106"/>
@@ -14958,7 +14961,7 @@
       <c r="S254" s="106"/>
       <c r="T254" s="106"/>
       <c r="U254" s="106" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="V254" s="106"/>
       <c r="W254" s="106"/>
@@ -15126,7 +15129,7 @@
       <c r="S260" s="106"/>
       <c r="T260" s="106"/>
       <c r="U260" s="106" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="V260" s="106"/>
       <c r="W260" s="106"/>
@@ -15266,7 +15269,7 @@
       <c r="S265" s="106"/>
       <c r="T265" s="106"/>
       <c r="U265" s="106" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="V265" s="106"/>
       <c r="W265" s="106"/>
@@ -15322,7 +15325,7 @@
       <c r="S267" s="106"/>
       <c r="T267" s="106"/>
       <c r="U267" s="106" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="V267" s="106"/>
       <c r="W267" s="106"/>
@@ -15518,7 +15521,7 @@
       <c r="S274" s="106"/>
       <c r="T274" s="106"/>
       <c r="U274" s="106" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="V274" s="106"/>
       <c r="W274" s="106"/>
@@ -15574,7 +15577,7 @@
       <c r="S276" s="106"/>
       <c r="T276" s="106"/>
       <c r="U276" s="106" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="V276" s="106"/>
       <c r="W276" s="106"/>
@@ -15602,7 +15605,7 @@
       <c r="S277" s="106"/>
       <c r="T277" s="106"/>
       <c r="U277" s="106" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="V277" s="106"/>
       <c r="W277" s="106"/>
@@ -15742,7 +15745,7 @@
       <c r="S282" s="106"/>
       <c r="T282" s="106"/>
       <c r="U282" s="106" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="V282" s="106"/>
       <c r="W282" s="106"/>
@@ -15770,7 +15773,7 @@
       <c r="S283" s="106"/>
       <c r="T283" s="106"/>
       <c r="U283" s="106" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="V283" s="106"/>
       <c r="W283" s="106"/>
@@ -16134,7 +16137,7 @@
       <c r="S296" s="106"/>
       <c r="T296" s="106"/>
       <c r="U296" s="106" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="V296" s="106"/>
       <c r="W296" s="106"/>
@@ -16190,7 +16193,7 @@
       <c r="S298" s="106"/>
       <c r="T298" s="106"/>
       <c r="U298" s="106" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="V298" s="106"/>
       <c r="W298" s="106"/>
@@ -16274,7 +16277,7 @@
       <c r="S301" s="106"/>
       <c r="T301" s="106"/>
       <c r="U301" s="106" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="V301" s="106"/>
       <c r="W301" s="106"/>
@@ -16302,7 +16305,7 @@
       <c r="S302" s="106"/>
       <c r="T302" s="106"/>
       <c r="U302" s="106" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="V302" s="106"/>
       <c r="W302" s="106"/>
@@ -16358,7 +16361,7 @@
       <c r="S304" s="106"/>
       <c r="T304" s="106"/>
       <c r="U304" s="106" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="V304" s="106"/>
       <c r="W304" s="106"/>
@@ -16442,7 +16445,7 @@
       <c r="S307" s="106"/>
       <c r="T307" s="106"/>
       <c r="U307" s="106" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="V307" s="106"/>
       <c r="W307" s="106"/>
@@ -16666,7 +16669,7 @@
       <c r="S315" s="106"/>
       <c r="T315" s="106"/>
       <c r="U315" s="106" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="V315" s="106"/>
       <c r="W315" s="106"/>
@@ -16750,7 +16753,7 @@
       <c r="S318" s="106"/>
       <c r="T318" s="106"/>
       <c r="U318" s="106" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="V318" s="106"/>
       <c r="W318" s="106"/>
@@ -16778,7 +16781,7 @@
       <c r="S319" s="106"/>
       <c r="T319" s="106"/>
       <c r="U319" s="106" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="V319" s="106"/>
       <c r="W319" s="106"/>
@@ -17030,7 +17033,7 @@
       <c r="S328" s="106"/>
       <c r="T328" s="106"/>
       <c r="U328" s="106" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="V328" s="106"/>
       <c r="W328" s="106"/>
@@ -17114,7 +17117,7 @@
       <c r="S331" s="106"/>
       <c r="T331" s="106"/>
       <c r="U331" s="106" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="V331" s="106"/>
       <c r="W331" s="106"/>
@@ -17170,7 +17173,7 @@
       <c r="S333" s="106"/>
       <c r="T333" s="106"/>
       <c r="U333" s="106" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="V333" s="106"/>
       <c r="W333" s="106"/>
@@ -17450,7 +17453,7 @@
       <c r="S343" s="106"/>
       <c r="T343" s="106"/>
       <c r="U343" s="106" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="V343" s="106"/>
       <c r="W343" s="106"/>
@@ -17478,7 +17481,7 @@
       <c r="S344" s="106"/>
       <c r="T344" s="106"/>
       <c r="U344" s="106" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="V344" s="106"/>
       <c r="W344" s="106"/>
@@ -17590,7 +17593,7 @@
       <c r="S348" s="106"/>
       <c r="T348" s="106"/>
       <c r="U348" s="106" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="V348" s="106"/>
       <c r="W348" s="106"/>
@@ -17618,7 +17621,7 @@
       <c r="S349" s="106"/>
       <c r="T349" s="106"/>
       <c r="U349" s="106" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="V349" s="106"/>
       <c r="W349" s="106"/>
@@ -17646,7 +17649,7 @@
       <c r="S350" s="106"/>
       <c r="T350" s="106"/>
       <c r="U350" s="106" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="V350" s="106"/>
       <c r="W350" s="106"/>
@@ -17758,7 +17761,7 @@
       <c r="S354" s="106"/>
       <c r="T354" s="106"/>
       <c r="U354" s="106" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="V354" s="106"/>
       <c r="W354" s="106"/>
@@ -17870,7 +17873,7 @@
       <c r="S358" s="106"/>
       <c r="T358" s="106"/>
       <c r="U358" s="106" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="V358" s="106"/>
       <c r="W358" s="106"/>
@@ -18038,7 +18041,7 @@
       <c r="S364" s="106"/>
       <c r="T364" s="106"/>
       <c r="U364" s="106" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="V364" s="106"/>
       <c r="W364" s="106"/>
@@ -18206,7 +18209,7 @@
       <c r="S370" s="106"/>
       <c r="T370" s="106"/>
       <c r="U370" s="106" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="V370" s="106"/>
       <c r="W370" s="106"/>
@@ -18234,7 +18237,7 @@
       <c r="S371" s="106"/>
       <c r="T371" s="106"/>
       <c r="U371" s="106" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="V371" s="106"/>
       <c r="W371" s="106"/>
@@ -18402,7 +18405,7 @@
       <c r="S377" s="106"/>
       <c r="T377" s="106"/>
       <c r="U377" s="106" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="V377" s="106"/>
       <c r="W377" s="106"/>
@@ -18458,7 +18461,7 @@
       <c r="S379" s="106"/>
       <c r="T379" s="106"/>
       <c r="U379" s="106" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="V379" s="106"/>
       <c r="W379" s="106"/>
@@ -18934,7 +18937,7 @@
       <c r="S396" s="106"/>
       <c r="T396" s="106"/>
       <c r="U396" s="106" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="V396" s="106"/>
       <c r="W396" s="106"/>
@@ -19046,7 +19049,7 @@
       <c r="S400" s="106"/>
       <c r="T400" s="106"/>
       <c r="U400" s="106" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="V400" s="106"/>
       <c r="W400" s="106"/>
@@ -19074,7 +19077,7 @@
       <c r="S401" s="106"/>
       <c r="T401" s="106"/>
       <c r="U401" s="106" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="V401" s="106"/>
       <c r="W401" s="106"/>
@@ -19130,7 +19133,7 @@
       <c r="S403" s="106"/>
       <c r="T403" s="106"/>
       <c r="U403" s="106" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="V403" s="106"/>
       <c r="W403" s="106"/>
@@ -19382,7 +19385,7 @@
       <c r="S412" s="106"/>
       <c r="T412" s="106"/>
       <c r="U412" s="106" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="V412" s="106"/>
       <c r="W412" s="106"/>
@@ -19410,7 +19413,7 @@
       <c r="S413" s="106"/>
       <c r="T413" s="106"/>
       <c r="U413" s="106" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="V413" s="106"/>
       <c r="W413" s="106"/>
@@ -19830,7 +19833,7 @@
       <c r="S428" s="106"/>
       <c r="T428" s="106"/>
       <c r="U428" s="106" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="V428" s="106"/>
       <c r="W428" s="106"/>
@@ -19886,7 +19889,7 @@
       <c r="S430" s="106"/>
       <c r="T430" s="106"/>
       <c r="U430" s="106" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="V430" s="106"/>
       <c r="W430" s="106"/>
@@ -20082,7 +20085,7 @@
       <c r="S437" s="106"/>
       <c r="T437" s="106"/>
       <c r="U437" s="106" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="V437" s="106"/>
       <c r="W437" s="106"/>
@@ -20334,7 +20337,7 @@
       <c r="S446" s="106"/>
       <c r="T446" s="106"/>
       <c r="U446" s="106" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="V446" s="106"/>
       <c r="W446" s="106"/>
@@ -20390,7 +20393,7 @@
       <c r="S448" s="106"/>
       <c r="T448" s="106"/>
       <c r="U448" s="106" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="V448" s="106"/>
       <c r="W448" s="106"/>
@@ -20642,7 +20645,7 @@
       <c r="S457" s="106"/>
       <c r="T457" s="106"/>
       <c r="U457" s="106" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="V457" s="106"/>
       <c r="W457" s="106"/>
@@ -20866,7 +20869,7 @@
       <c r="S465" s="106"/>
       <c r="T465" s="106"/>
       <c r="U465" s="106" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="V465" s="106"/>
       <c r="W465" s="106"/>
@@ -21146,7 +21149,7 @@
       <c r="S475" s="106"/>
       <c r="T475" s="106"/>
       <c r="U475" s="106" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="V475" s="106"/>
       <c r="W475" s="106"/>
@@ -21174,7 +21177,7 @@
       <c r="S476" s="106"/>
       <c r="T476" s="106"/>
       <c r="U476" s="106" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="V476" s="106"/>
       <c r="W476" s="106"/>
@@ -21619,23 +21622,23 @@
     <sortCondition ref="T5"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="70">
-      <selection activeCell="H4" sqref="H4"/>
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="80" topLeftCell="E1">
+      <selection activeCell="I21" sqref="I21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="80" topLeftCell="A2">
+      <selection activeCell="L8" sqref="L8"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="80" topLeftCell="C1">
       <selection activeCell="F5" sqref="F5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="80" topLeftCell="A2">
-      <selection activeCell="L8" sqref="L8"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="80" topLeftCell="E1">
-      <selection activeCell="I21" sqref="I21"/>
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="70">
+      <selection activeCell="H4" sqref="H4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -21670,7 +21673,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="87" t="s">
-        <v>1275</v>
+        <v>1268</v>
       </c>
       <c r="C1" s="87" t="s">
         <v>617</v>
@@ -21679,7 +21682,7 @@
         <v>618</v>
       </c>
       <c r="E1" s="87" t="s">
-        <v>1283</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -21771,16 +21774,16 @@
         <v>15</v>
       </c>
       <c r="B8" s="95" t="s">
-        <v>1276</v>
+        <v>1269</v>
       </c>
       <c r="C8" s="95" t="s">
-        <v>1273</v>
+        <v>1266</v>
       </c>
       <c r="D8" s="95" t="s">
-        <v>1274</v>
+        <v>1267</v>
       </c>
       <c r="E8" s="95" t="s">
-        <v>1284</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="113" customFormat="1" x14ac:dyDescent="0.2">
@@ -21789,13 +21792,13 @@
         <v>58</v>
       </c>
       <c r="C9" s="114" t="s">
-        <v>1279</v>
+        <v>1272</v>
       </c>
       <c r="D9" s="114" t="s">
-        <v>1280</v>
+        <v>1273</v>
       </c>
       <c r="E9" s="119" t="s">
-        <v>1285</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -21804,13 +21807,13 @@
         <v>58</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>1281</v>
+        <v>1274</v>
       </c>
       <c r="D10" s="75" t="s">
-        <v>1282</v>
+        <v>1275</v>
       </c>
       <c r="E10" s="120" t="s">
-        <v>1286</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -21829,25 +21832,25 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="55" showGridLines="0">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="55" showGridLines="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="80" showGridLines="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+    </customSheetView>
     <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="55" showGridLines="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="80" showGridLines="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="55" showGridLines="0">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="55" showGridLines="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21877,8 +21880,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -21903,25 +21906,25 @@
         <v>NORTHING</v>
       </c>
       <c r="E1" s="87" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="F1" s="87" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="G1" s="87" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="H1" s="87" t="s">
         <v>58</v>
       </c>
       <c r="I1" s="87" t="s">
-        <v>1185</v>
+        <v>1182</v>
       </c>
       <c r="J1" s="87" t="s">
         <v>616</v>
       </c>
       <c r="K1" s="87" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
       <c r="L1" s="87" t="s">
         <v>647</v>
@@ -21936,16 +21939,16 @@
         <v>539</v>
       </c>
       <c r="P1" s="87" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="Q1" s="87" t="s">
-        <v>1287</v>
+        <v>1280</v>
       </c>
       <c r="R1" s="87" t="s">
         <v>594</v>
       </c>
       <c r="S1" s="87" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="T1" s="87" t="s">
         <v>2</v>
@@ -21972,7 +21975,7 @@
       </c>
       <c r="G2" s="96"/>
       <c r="H2" s="96" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="I2" s="96" t="s">
         <v>66</v>
@@ -22002,7 +22005,7 @@
         <v>542</v>
       </c>
       <c r="T2" s="96" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="25.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -22329,28 +22332,28 @@
         <v>NORTHING: Y offet from the UTM zone point of origin in metres</v>
       </c>
       <c r="E8" s="95" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="F8" s="95" t="s">
         <v>639</v>
       </c>
       <c r="G8" s="95" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="H8" s="95" t="s">
-        <v>1252</v>
+        <v>1249</v>
       </c>
       <c r="I8" s="95" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="J8" s="95" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="K8" s="95" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="L8" s="95" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="M8" s="95" t="s">
         <v>194</v>
@@ -22359,19 +22362,19 @@
         <v>195</v>
       </c>
       <c r="O8" s="95" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="P8" s="95" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="Q8" s="95" t="s">
-        <v>1203</v>
+        <v>1200</v>
       </c>
       <c r="R8" s="95" t="s">
         <v>541</v>
       </c>
       <c r="S8" s="95" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="T8" s="95" t="s">
         <v>16</v>
@@ -22380,7 +22383,7 @@
     <row r="9" spans="1:20" s="101" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="100"/>
       <c r="B9" s="98" t="s">
-        <v>1201</v>
+        <v>1198</v>
       </c>
       <c r="C9" s="111">
         <v>123456</v>
@@ -22396,10 +22399,10 @@
       </c>
       <c r="G9" s="111"/>
       <c r="H9" s="98" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="I9" s="98" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="J9" s="116">
         <v>-60</v>
@@ -22408,7 +22411,7 @@
         <v>270</v>
       </c>
       <c r="L9" s="98" t="s">
-        <v>648</v>
+        <v>1281</v>
       </c>
       <c r="M9" s="102">
         <v>36526</v>
@@ -22420,23 +22423,23 @@
         <v>596</v>
       </c>
       <c r="P9" s="98" t="s">
-        <v>1199</v>
+        <v>1196</v>
       </c>
       <c r="Q9" s="98" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="R9" s="103">
         <v>3</v>
       </c>
       <c r="S9" s="98" t="s">
-        <v>1202</v>
+        <v>1199</v>
       </c>
       <c r="T9" s="98"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="6" t="s">
-        <v>1270</v>
+        <v>1263</v>
       </c>
       <c r="C10" s="75">
         <v>123456</v>
@@ -22452,10 +22455,10 @@
       </c>
       <c r="G10" s="76"/>
       <c r="H10" s="6" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>1176</v>
+        <v>1173</v>
       </c>
       <c r="J10" s="77">
         <v>-60</v>
@@ -22464,7 +22467,7 @@
         <v>270</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>649</v>
+        <v>1282</v>
       </c>
       <c r="M10" s="78">
         <v>45179</v>
@@ -22476,14 +22479,14 @@
         <v>596</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>1271</v>
+        <v>1264</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>1200</v>
+        <v>1197</v>
       </c>
       <c r="R10" s="45"/>
       <c r="S10" s="6" t="s">
-        <v>1272</v>
+        <v>1265</v>
       </c>
       <c r="T10" s="6"/>
     </row>
@@ -22643,23 +22646,23 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="60" showGridLines="0" topLeftCell="D1">
-      <selection activeCell="J13" sqref="J13"/>
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="60" showGridLines="0" topLeftCell="G1">
+      <selection activeCell="C12" sqref="C12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="80" showGridLines="0">
+      <selection activeCell="G1" sqref="G1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="60" showGridLines="0">
       <selection activeCell="E3" sqref="E3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="80" showGridLines="0">
-      <selection activeCell="G1" sqref="G1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="60" showGridLines="0" topLeftCell="G1">
-      <selection activeCell="C12" sqref="C12"/>
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="60" showGridLines="0" topLeftCell="D1">
+      <selection activeCell="J13" sqref="J13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -25499,22 +25502,22 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" state="hidden">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" state="hidden">
       <selection activeCell="F21" sqref="F21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" state="hidden">
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" state="hidden">
       <selection activeCell="F21" sqref="F21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" state="hidden">
+    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" state="hidden">
       <selection activeCell="F21" sqref="F21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" state="hidden">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" state="hidden">
       <selection activeCell="F21" sqref="F21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -29185,22 +29188,22 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" state="hidden">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" state="hidden">
       <selection activeCell="C5" sqref="C5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" state="hidden">
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" state="hidden">
       <selection activeCell="C5" sqref="C5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" state="hidden">
+    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" state="hidden">
       <selection activeCell="C5" sqref="C5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" state="hidden">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" state="hidden">
       <selection activeCell="C5" sqref="C5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -36199,22 +36202,22 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" hiddenColumns="1" state="hidden">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" hiddenColumns="1" state="hidden">
       <selection activeCell="P9" activeCellId="1" sqref="G9 P9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" hiddenColumns="1" state="hidden">
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" hiddenColumns="1" state="hidden">
       <selection activeCell="P9" activeCellId="1" sqref="G9 P9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" hiddenColumns="1" state="hidden">
+    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" hiddenColumns="1" state="hidden">
       <selection activeCell="P9" activeCellId="1" sqref="G9 P9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" hiddenColumns="1" state="hidden">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" hiddenColumns="1" state="hidden">
       <selection activeCell="P9" activeCellId="1" sqref="G9 P9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -44291,22 +44294,22 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
       <selection activeCell="Q1" activeCellId="3" sqref="A1:A65536 H1:H65536 L1:N65536 Q1:V65536"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
       <selection activeCell="Q1" activeCellId="3" sqref="A1:A65536 H1:H65536 L1:N65536 Q1:V65536"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
+    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
       <selection activeCell="Q1" activeCellId="3" sqref="A1:A65536 H1:H65536 L1:N65536 Q1:V65536"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
       <selection activeCell="Q1" activeCellId="3" sqref="A1:A65536 H1:H65536 L1:N65536 Q1:V65536"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -44829,25 +44832,25 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <customSheetViews>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -44877,20 +44880,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <AssignedTo xmlns="cc9fd5b5-cf46-4eda-9201-7118bc1c1603">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </AssignedTo>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006CE8352A0AF1CD4AB9B3521FB05BB06E" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fe27245e9bb914202a9dc14def4cd737">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cc9fd5b5-cf46-4eda-9201-7118bc1c1603" xmlns:ns3="bcd33c6e-30cb-4633-b8ec-d716de95c77b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b8902f26a47aaca738f2017df961ee0" ns2:_="" ns3:_="">
     <xsd:import namespace="cc9fd5b5-cf46-4eda-9201-7118bc1c1603"/>
@@ -45121,6 +45110,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <AssignedTo xmlns="cc9fd5b5-cf46-4eda-9201-7118bc1c1603">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </AssignedTo>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -45131,23 +45134,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9C12B8D-B909-479A-8F46-E01C349A93B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="bcd33c6e-30cb-4633-b8ec-d716de95c77b"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cc9fd5b5-cf46-4eda-9201-7118bc1c1603"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF79EA6D-2196-4B94-BF37-7CE4AD2619E6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -45166,6 +45152,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9C12B8D-B909-479A-8F46-E01C349A93B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="bcd33c6e-30cb-4633-b8ec-d716de95c77b"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cc9fd5b5-cf46-4eda-9201-7118bc1c1603"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CEE68A9-1E3D-4013-A8AF-E88F960C4957}">
   <ds:schemaRefs>

</xml_diff>